<commit_message>
Added functions to save data from JXTable into excel file with right number format. Added some testing classes for Joptionpane to display a proper dialog message.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="91">
   <si>
     <t>3</t>
   </si>
@@ -261,20 +261,366 @@
   </si>
   <si>
     <t>ΦΠΑ</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Ημερομηνία</t>
+  </si>
+  <si>
+    <t>Κατηγορία</t>
+  </si>
+  <si>
+    <t>Έσοδο/Έξοδο</t>
+  </si>
+  <si>
+    <t>Ποσό(€)</t>
+  </si>
+  <si>
+    <t>Αιτιολογία</t>
+  </si>
+  <si>
+    <t>Παραδόσεις</t>
+  </si>
+  <si>
+    <t>Παραλαβές</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyy"/>
+  </numFmts>
+  <fonts count="65">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -297,8 +643,444 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="437">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -311,43 +1093,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.14453125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="6.55859375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.91015625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="6.9609375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="5.85546875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.94921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.19140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="3.14453125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="3.14453125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.40234375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.75" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.09375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.94921875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.2421875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.57421875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="n">
-        <v>42396.0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1"/>
-      <c r="H1"/>
+      <c r="A1" t="s" s="392">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s" s="393">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s" s="394">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s" s="395">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s" s="396">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s" s="397">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s" s="398">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s" s="399">
+        <v>90</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B2" t="n" s="400">
         <v>42391.0</v>
       </c>
       <c r="C2" t="s">
@@ -366,10 +1152,10 @@
       <c r="H2"/>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B3" t="n" s="401">
         <v>42397.0</v>
       </c>
       <c r="C3" t="s">
@@ -388,10 +1174,10 @@
       <c r="H3"/>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n" s="402">
         <v>42396.0</v>
       </c>
       <c r="C4" t="s">
@@ -414,10 +1200,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="n">
+      <c r="A5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B5" t="n" s="403">
         <v>42397.0</v>
       </c>
       <c r="C5" t="s">
@@ -440,10 +1226,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="A6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B6" t="n" s="404">
         <v>42393.0</v>
       </c>
       <c r="C6" t="s">
@@ -466,10 +1252,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="n">
+      <c r="A7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B7" t="n" s="405">
         <v>42394.0</v>
       </c>
       <c r="C7" t="s">
@@ -492,10 +1278,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="n">
+      <c r="A8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B8" t="n" s="406">
         <v>42395.0</v>
       </c>
       <c r="C8" t="s">
@@ -518,10 +1304,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="n">
+      <c r="A9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B9" t="n" s="407">
         <v>42358.0</v>
       </c>
       <c r="C9" t="s">
@@ -544,10 +1330,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="n">
+      <c r="A10" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B10" t="n" s="408">
         <v>42359.0</v>
       </c>
       <c r="C10" t="s">
@@ -570,10 +1356,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="n">
+      <c r="A11" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B11" t="n" s="409">
         <v>42360.0</v>
       </c>
       <c r="C11" t="s">
@@ -596,10 +1382,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="n">
+      <c r="A12" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B12" t="n" s="410">
         <v>42361.0</v>
       </c>
       <c r="C12" t="s">
@@ -622,10 +1408,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="n">
+      <c r="A13" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B13" t="n" s="411">
         <v>42362.0</v>
       </c>
       <c r="C13" t="s">
@@ -648,10 +1434,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" t="n">
+      <c r="A14" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B14" t="n" s="412">
         <v>42363.0</v>
       </c>
       <c r="C14" t="s">
@@ -674,10 +1460,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="n">
+      <c r="A15" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B15" t="n" s="413">
         <v>42364.0</v>
       </c>
       <c r="C15" t="s">
@@ -700,10 +1486,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="n">
+      <c r="A16" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B16" t="n" s="414">
         <v>42365.0</v>
       </c>
       <c r="C16" t="s">
@@ -726,10 +1512,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" t="n">
+      <c r="A17" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B17" t="n" s="415">
         <v>42366.0</v>
       </c>
       <c r="C17" t="s">
@@ -752,10 +1538,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="n">
+      <c r="A18" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B18" t="n" s="416">
         <v>42367.0</v>
       </c>
       <c r="C18" t="s">
@@ -778,10 +1564,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="n">
+      <c r="A19" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B19" t="n" s="417">
         <v>42368.0</v>
       </c>
       <c r="C19" t="s">
@@ -804,10 +1590,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="n">
+      <c r="A20" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B20" t="n" s="418">
         <v>42369.0</v>
       </c>
       <c r="C20" t="s">
@@ -830,10 +1616,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="n">
+      <c r="A21" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B21" t="n" s="419">
         <v>42370.0</v>
       </c>
       <c r="C21" t="s">
@@ -856,10 +1642,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" t="n">
+      <c r="A22" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B22" t="n" s="420">
         <v>42371.0</v>
       </c>
       <c r="C22" t="s">
@@ -882,10 +1668,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="n">
+      <c r="A23" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B23" t="n" s="421">
         <v>42372.0</v>
       </c>
       <c r="C23" t="s">
@@ -908,10 +1694,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" t="n">
+      <c r="A24" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B24" t="n" s="422">
         <v>42373.0</v>
       </c>
       <c r="C24" t="s">
@@ -934,10 +1720,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" t="n">
+      <c r="A25" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B25" t="n" s="423">
         <v>42374.0</v>
       </c>
       <c r="C25" t="s">
@@ -960,10 +1746,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="n">
+      <c r="A26" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B26" t="n" s="424">
         <v>42396.0</v>
       </c>
       <c r="C26" t="s">
@@ -982,10 +1768,10 @@
       <c r="H26"/>
     </row>
     <row r="27">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" t="n">
+      <c r="A27" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B27" t="n" s="425">
         <v>42397.0</v>
       </c>
       <c r="C27" t="s">
@@ -1004,10 +1790,10 @@
       <c r="H27"/>
     </row>
     <row r="28">
-      <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" t="n">
+      <c r="A28" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B28" t="n" s="426">
         <v>42395.0</v>
       </c>
       <c r="C28" t="s">
@@ -1026,10 +1812,10 @@
       <c r="H28"/>
     </row>
     <row r="29">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" t="n">
+      <c r="A29" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B29" t="n" s="427">
         <v>42394.0</v>
       </c>
       <c r="C29" t="s">
@@ -1048,10 +1834,10 @@
       <c r="H29"/>
     </row>
     <row r="30">
-      <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" t="n">
+      <c r="A30" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B30" t="n" s="428">
         <v>42393.0</v>
       </c>
       <c r="C30" t="s">
@@ -1070,10 +1856,10 @@
       <c r="H30"/>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" t="n">
+      <c r="A31" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B31" t="n" s="429">
         <v>42393.0</v>
       </c>
       <c r="C31" t="s">
@@ -1092,10 +1878,10 @@
       <c r="H31"/>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" t="n">
+      <c r="A32" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B32" t="n" s="430">
         <v>42394.0</v>
       </c>
       <c r="C32" t="s">
@@ -1114,10 +1900,10 @@
       <c r="H32"/>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" t="n">
+      <c r="A33" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B33" t="n" s="431">
         <v>42395.0</v>
       </c>
       <c r="C33" t="s">
@@ -1136,10 +1922,10 @@
       <c r="H33"/>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" t="n">
+      <c r="A34" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B34" t="n" s="432">
         <v>42396.0</v>
       </c>
       <c r="C34" t="s">
@@ -1158,10 +1944,10 @@
       <c r="H34"/>
     </row>
     <row r="35">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" t="n">
+      <c r="A35" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B35" t="n" s="433">
         <v>42366.0</v>
       </c>
       <c r="C35" t="s">
@@ -1180,10 +1966,10 @@
       <c r="H35"/>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" t="n">
+      <c r="A36" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B36" t="n" s="434">
         <v>42394.0</v>
       </c>
       <c r="C36" t="s">
@@ -1202,10 +1988,10 @@
       <c r="H36"/>
     </row>
     <row r="37">
-      <c r="A37" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" t="n">
+      <c r="A37" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B37" t="n" s="435">
         <v>42397.0</v>
       </c>
       <c r="C37" t="s">
@@ -1224,10 +2010,10 @@
       <c r="H37"/>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" t="n">
+      <c r="A38" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B38" t="n" s="436">
         <v>42365.0</v>
       </c>
       <c r="C38" t="s">

</xml_diff>

<commit_message>
NEW: When u click at Save Excel... Menu Item will now open a JFileChooser to choose where the file will be save. Added a Test class to test the JFileChooser to work poperly
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2302" uniqueCount="91">
   <si>
     <t>3</t>
   </si>
@@ -294,7 +294,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="dd/mm/yyy"/>
   </numFmts>
-  <fonts count="65">
+  <fonts count="97">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -340,6 +340,166 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
       <b val="true"/>
     </font>
     <font>
@@ -643,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="437">
+  <cellXfs count="617">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -1044,6 +1204,186 @@
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -1104,28 +1444,28 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="392">
+      <c r="A1" t="s" s="572">
         <v>83</v>
       </c>
-      <c r="B1" t="s" s="393">
+      <c r="B1" t="s" s="573">
         <v>84</v>
       </c>
-      <c r="C1" t="s" s="394">
+      <c r="C1" t="s" s="574">
         <v>85</v>
       </c>
-      <c r="D1" t="s" s="395">
+      <c r="D1" t="s" s="575">
         <v>86</v>
       </c>
-      <c r="E1" t="s" s="396">
+      <c r="E1" t="s" s="576">
         <v>87</v>
       </c>
-      <c r="F1" t="s" s="397">
+      <c r="F1" t="s" s="577">
         <v>88</v>
       </c>
-      <c r="G1" t="s" s="398">
+      <c r="G1" t="s" s="578">
         <v>89</v>
       </c>
-      <c r="H1" t="s" s="399">
+      <c r="H1" t="s" s="579">
         <v>90</v>
       </c>
     </row>
@@ -1133,7 +1473,7 @@
       <c r="A2" t="n">
         <v>4.0</v>
       </c>
-      <c r="B2" t="n" s="400">
+      <c r="B2" t="n" s="580">
         <v>42391.0</v>
       </c>
       <c r="C2" t="s">
@@ -1155,7 +1495,7 @@
       <c r="A3" t="n">
         <v>5.0</v>
       </c>
-      <c r="B3" t="n" s="401">
+      <c r="B3" t="n" s="581">
         <v>42397.0</v>
       </c>
       <c r="C3" t="s">
@@ -1177,7 +1517,7 @@
       <c r="A4" t="n">
         <v>1.0</v>
       </c>
-      <c r="B4" t="n" s="402">
+      <c r="B4" t="n" s="582">
         <v>42396.0</v>
       </c>
       <c r="C4" t="s">
@@ -1203,7 +1543,7 @@
       <c r="A5" t="n">
         <v>2.0</v>
       </c>
-      <c r="B5" t="n" s="403">
+      <c r="B5" t="n" s="583">
         <v>42397.0</v>
       </c>
       <c r="C5" t="s">
@@ -1229,7 +1569,7 @@
       <c r="A6" t="n">
         <v>3.0</v>
       </c>
-      <c r="B6" t="n" s="404">
+      <c r="B6" t="n" s="584">
         <v>42393.0</v>
       </c>
       <c r="C6" t="s">
@@ -1255,7 +1595,7 @@
       <c r="A7" t="n">
         <v>4.0</v>
       </c>
-      <c r="B7" t="n" s="405">
+      <c r="B7" t="n" s="585">
         <v>42394.0</v>
       </c>
       <c r="C7" t="s">
@@ -1281,7 +1621,7 @@
       <c r="A8" t="n">
         <v>5.0</v>
       </c>
-      <c r="B8" t="n" s="406">
+      <c r="B8" t="n" s="586">
         <v>42395.0</v>
       </c>
       <c r="C8" t="s">
@@ -1307,7 +1647,7 @@
       <c r="A9" t="n">
         <v>6.0</v>
       </c>
-      <c r="B9" t="n" s="407">
+      <c r="B9" t="n" s="587">
         <v>42358.0</v>
       </c>
       <c r="C9" t="s">
@@ -1333,7 +1673,7 @@
       <c r="A10" t="n">
         <v>7.0</v>
       </c>
-      <c r="B10" t="n" s="408">
+      <c r="B10" t="n" s="588">
         <v>42359.0</v>
       </c>
       <c r="C10" t="s">
@@ -1359,7 +1699,7 @@
       <c r="A11" t="n">
         <v>8.0</v>
       </c>
-      <c r="B11" t="n" s="409">
+      <c r="B11" t="n" s="589">
         <v>42360.0</v>
       </c>
       <c r="C11" t="s">
@@ -1385,7 +1725,7 @@
       <c r="A12" t="n">
         <v>9.0</v>
       </c>
-      <c r="B12" t="n" s="410">
+      <c r="B12" t="n" s="590">
         <v>42361.0</v>
       </c>
       <c r="C12" t="s">
@@ -1411,7 +1751,7 @@
       <c r="A13" t="n">
         <v>10.0</v>
       </c>
-      <c r="B13" t="n" s="411">
+      <c r="B13" t="n" s="591">
         <v>42362.0</v>
       </c>
       <c r="C13" t="s">
@@ -1437,7 +1777,7 @@
       <c r="A14" t="n">
         <v>11.0</v>
       </c>
-      <c r="B14" t="n" s="412">
+      <c r="B14" t="n" s="592">
         <v>42363.0</v>
       </c>
       <c r="C14" t="s">
@@ -1463,7 +1803,7 @@
       <c r="A15" t="n">
         <v>12.0</v>
       </c>
-      <c r="B15" t="n" s="413">
+      <c r="B15" t="n" s="593">
         <v>42364.0</v>
       </c>
       <c r="C15" t="s">
@@ -1489,7 +1829,7 @@
       <c r="A16" t="n">
         <v>13.0</v>
       </c>
-      <c r="B16" t="n" s="414">
+      <c r="B16" t="n" s="594">
         <v>42365.0</v>
       </c>
       <c r="C16" t="s">
@@ -1515,7 +1855,7 @@
       <c r="A17" t="n">
         <v>14.0</v>
       </c>
-      <c r="B17" t="n" s="415">
+      <c r="B17" t="n" s="595">
         <v>42366.0</v>
       </c>
       <c r="C17" t="s">
@@ -1541,7 +1881,7 @@
       <c r="A18" t="n">
         <v>15.0</v>
       </c>
-      <c r="B18" t="n" s="416">
+      <c r="B18" t="n" s="596">
         <v>42367.0</v>
       </c>
       <c r="C18" t="s">
@@ -1567,7 +1907,7 @@
       <c r="A19" t="n">
         <v>16.0</v>
       </c>
-      <c r="B19" t="n" s="417">
+      <c r="B19" t="n" s="597">
         <v>42368.0</v>
       </c>
       <c r="C19" t="s">
@@ -1593,7 +1933,7 @@
       <c r="A20" t="n">
         <v>17.0</v>
       </c>
-      <c r="B20" t="n" s="418">
+      <c r="B20" t="n" s="598">
         <v>42369.0</v>
       </c>
       <c r="C20" t="s">
@@ -1619,7 +1959,7 @@
       <c r="A21" t="n">
         <v>18.0</v>
       </c>
-      <c r="B21" t="n" s="419">
+      <c r="B21" t="n" s="599">
         <v>42370.0</v>
       </c>
       <c r="C21" t="s">
@@ -1645,7 +1985,7 @@
       <c r="A22" t="n">
         <v>19.0</v>
       </c>
-      <c r="B22" t="n" s="420">
+      <c r="B22" t="n" s="600">
         <v>42371.0</v>
       </c>
       <c r="C22" t="s">
@@ -1671,7 +2011,7 @@
       <c r="A23" t="n">
         <v>20.0</v>
       </c>
-      <c r="B23" t="n" s="421">
+      <c r="B23" t="n" s="601">
         <v>42372.0</v>
       </c>
       <c r="C23" t="s">
@@ -1697,7 +2037,7 @@
       <c r="A24" t="n">
         <v>21.0</v>
       </c>
-      <c r="B24" t="n" s="422">
+      <c r="B24" t="n" s="602">
         <v>42373.0</v>
       </c>
       <c r="C24" t="s">
@@ -1723,7 +2063,7 @@
       <c r="A25" t="n">
         <v>22.0</v>
       </c>
-      <c r="B25" t="n" s="423">
+      <c r="B25" t="n" s="603">
         <v>42374.0</v>
       </c>
       <c r="C25" t="s">
@@ -1749,7 +2089,7 @@
       <c r="A26" t="n">
         <v>3.0</v>
       </c>
-      <c r="B26" t="n" s="424">
+      <c r="B26" t="n" s="604">
         <v>42396.0</v>
       </c>
       <c r="C26" t="s">
@@ -1771,7 +2111,7 @@
       <c r="A27" t="n">
         <v>4.0</v>
       </c>
-      <c r="B27" t="n" s="425">
+      <c r="B27" t="n" s="605">
         <v>42397.0</v>
       </c>
       <c r="C27" t="s">
@@ -1793,7 +2133,7 @@
       <c r="A28" t="n">
         <v>7.0</v>
       </c>
-      <c r="B28" t="n" s="426">
+      <c r="B28" t="n" s="606">
         <v>42395.0</v>
       </c>
       <c r="C28" t="s">
@@ -1815,7 +2155,7 @@
       <c r="A29" t="n">
         <v>8.0</v>
       </c>
-      <c r="B29" t="n" s="427">
+      <c r="B29" t="n" s="607">
         <v>42394.0</v>
       </c>
       <c r="C29" t="s">
@@ -1837,7 +2177,7 @@
       <c r="A30" t="n">
         <v>9.0</v>
       </c>
-      <c r="B30" t="n" s="428">
+      <c r="B30" t="n" s="608">
         <v>42393.0</v>
       </c>
       <c r="C30" t="s">
@@ -1859,7 +2199,7 @@
       <c r="A31" t="n">
         <v>10.0</v>
       </c>
-      <c r="B31" t="n" s="429">
+      <c r="B31" t="n" s="609">
         <v>42393.0</v>
       </c>
       <c r="C31" t="s">
@@ -1881,7 +2221,7 @@
       <c r="A32" t="n">
         <v>11.0</v>
       </c>
-      <c r="B32" t="n" s="430">
+      <c r="B32" t="n" s="610">
         <v>42394.0</v>
       </c>
       <c r="C32" t="s">
@@ -1903,7 +2243,7 @@
       <c r="A33" t="n">
         <v>12.0</v>
       </c>
-      <c r="B33" t="n" s="431">
+      <c r="B33" t="n" s="611">
         <v>42395.0</v>
       </c>
       <c r="C33" t="s">
@@ -1925,7 +2265,7 @@
       <c r="A34" t="n">
         <v>13.0</v>
       </c>
-      <c r="B34" t="n" s="432">
+      <c r="B34" t="n" s="612">
         <v>42396.0</v>
       </c>
       <c r="C34" t="s">
@@ -1947,7 +2287,7 @@
       <c r="A35" t="n">
         <v>14.0</v>
       </c>
-      <c r="B35" t="n" s="433">
+      <c r="B35" t="n" s="613">
         <v>42366.0</v>
       </c>
       <c r="C35" t="s">
@@ -1969,7 +2309,7 @@
       <c r="A36" t="n">
         <v>15.0</v>
       </c>
-      <c r="B36" t="n" s="434">
+      <c r="B36" t="n" s="614">
         <v>42394.0</v>
       </c>
       <c r="C36" t="s">
@@ -1991,7 +2331,7 @@
       <c r="A37" t="n">
         <v>16.0</v>
       </c>
-      <c r="B37" t="n" s="435">
+      <c r="B37" t="n" s="615">
         <v>42397.0</v>
       </c>
       <c r="C37" t="s">
@@ -2013,7 +2353,7 @@
       <c r="A38" t="n">
         <v>17.0</v>
       </c>
-      <c r="B38" t="n" s="436">
+      <c r="B38" t="n" s="616">
         <v>42365.0</v>
       </c>
       <c r="C38" t="s">

</xml_diff>